<commit_message>
Dr. E version from 2019-06-04
</commit_message>
<xml_diff>
--- a/fix_loc_global.xlsx
+++ b/fix_loc_global.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCOOK\Documents\Google Drive\Math\UN project\UN-Data-Mapping-copy\Network Project\new fix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne's  PC\Documents\Academic Positions\Tarleton State\2019\Summer 2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{992E4324-46E0-4DD6-8701-F0DA22DDC0CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="missing_loc_1.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -627,7 +628,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -942,7 +943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -953,13 +954,13 @@
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>199</v>
       </c>
@@ -967,7 +968,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -983,7 +984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -991,7 +992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1023,7 +1024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1079,7 +1080,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1087,7 +1088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1111,7 +1112,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1159,7 +1160,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1175,7 +1176,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
@@ -1207,7 +1208,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
@@ -1223,7 +1224,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -1231,7 +1232,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
@@ -1247,7 +1248,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
@@ -1255,7 +1256,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
@@ -1263,7 +1264,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>74</v>
       </c>
@@ -1271,7 +1272,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>78</v>
       </c>
@@ -1287,7 +1288,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
@@ -1303,7 +1304,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -1319,7 +1320,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>96</v>
       </c>
@@ -1359,7 +1360,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -1367,7 +1368,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
@@ -1375,7 +1376,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>102</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
@@ -1391,7 +1392,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>106</v>
       </c>
@@ -1399,7 +1400,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>109</v>
       </c>
@@ -1415,7 +1416,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>111</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>113</v>
       </c>
@@ -1431,7 +1432,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>114</v>
       </c>
@@ -1439,7 +1440,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
@@ -1447,7 +1448,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>118</v>
       </c>
@@ -1455,7 +1456,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>120</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>122</v>
       </c>
@@ -1471,7 +1472,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>124</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>126</v>
       </c>
@@ -1487,7 +1488,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>128</v>
       </c>
@@ -1495,7 +1496,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>130</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>132</v>
       </c>
@@ -1511,7 +1512,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>134</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>136</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>138</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>140</v>
       </c>
@@ -1543,7 +1544,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>142</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>144</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>146</v>
       </c>
@@ -1567,7 +1568,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>148</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>149</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>151</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>153</v>
       </c>
@@ -1599,7 +1600,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>155</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>157</v>
       </c>
@@ -1615,7 +1616,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>159</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>161</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>163</v>
       </c>
@@ -1639,7 +1640,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>165</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>167</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>169</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>171</v>
       </c>
@@ -1671,7 +1672,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>173</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>175</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>177</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>179</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>181</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>183</v>
       </c>
@@ -1719,7 +1720,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>184</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>186</v>
       </c>
@@ -1735,7 +1736,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>187</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>189</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>191</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>193</v>
       </c>
@@ -1767,7 +1768,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>195</v>
       </c>
@@ -1775,7 +1776,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>197</v>
       </c>

</xml_diff>